<commit_message>
20180301Th - ODS version of the Excel file
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/val/ESPD_Schematron v2.0.2.xlsx
+++ b/docs/src/main/asciidoc/dist/val/ESPD_Schematron v2.0.2.xlsx
@@ -4418,15 +4418,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D6C5B8CC32BC1140B6F0C5F77127AF3D" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="50657e288e8542fef45c07c828c745a3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="12d6af70-178b-4e5d-9119-f14160711e65" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b6d74b87087f25a4d98723b87f6102f7" ns2:_="">
     <xsd:import namespace="12d6af70-178b-4e5d-9119-f14160711e65"/>
@@ -4558,6 +4549,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4565,14 +4565,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70F527B5-3861-4669-BF6A-5F60B023FB7A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17441034-4EE2-4A3F-A633-5CC493B7426B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4590,6 +4582,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70F527B5-3861-4669-BF6A-5F60B023FB7A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E819421D-622A-4A07-A76D-B383825A21D6}">
   <ds:schemaRefs>

</xml_diff>